<commit_message>
Commit 3 - Performed Aggregation Function and Pipeline
</commit_message>
<xml_diff>
--- a/Workload.xlsx
+++ b/Workload.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STUDY\Desktop\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51434A3F-4BB5-4857-BF78-40C4FB13879B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CF2563-0DFB-4F7C-8845-D954EE60E550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workload" sheetId="1" r:id="rId1"/>
@@ -20,42 +20,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>Common Queries</t>
-  </si>
-  <si>
-    <t>Workload</t>
-  </si>
-  <si>
-    <t>Find documents by ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+  <si>
+    <t>Entities</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Information Needed</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Find by field</t>
+  </si>
+  <si>
+    <t>Field: name</t>
   </si>
   <si>
     <t>Read-heavy</t>
   </si>
   <si>
-    <t>Find documents by field</t>
-  </si>
-  <si>
-    <t>Insert a new document</t>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Insert new document</t>
   </si>
   <si>
     <t>Write-heavy</t>
   </si>
   <si>
-    <t>Update a document</t>
+    <t>ProductionLines</t>
+  </si>
+  <si>
+    <t>Update document</t>
+  </si>
+  <si>
+    <t>ProductionTasks</t>
   </si>
   <si>
     <t>Aggregate data</t>
   </si>
   <si>
+    <t>Pipeline stages for aggregation</t>
+  </si>
+  <si>
     <t>Mixed</t>
+  </si>
+  <si>
+    <t>Fields: name, category, unit_price</t>
+  </si>
+  <si>
+    <t>Filter criteria: _id, Field to update: status</t>
+  </si>
+  <si>
+    <t>Find by objectID</t>
+  </si>
+  <si>
+    <t>Field: _id</t>
+  </si>
+  <si>
+    <t>Indexed Fields</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Single Field Index</t>
+  </si>
+  <si>
+    <t>Index Type</t>
+  </si>
+  <si>
+    <t>No Index Needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,63 +940,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>